<commit_message>
count male female fhsis
</commit_message>
<xml_diff>
--- a/storage/AR_TEMPLATE.xlsx
+++ b/storage/AR_TEMPLATE.xlsx
@@ -1,26 +1,40 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27702"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\laragon\www\nrpcp\storage\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\laragon\www\cesu\storage\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C203AB1-6424-41D1-8E05-43B9A44F8241}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="MAIN" sheetId="16" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <fileRecoveryPr autoRecover="0"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="40">
   <si>
     <t>Rabies Prevention and Control Program</t>
   </si>
@@ -140,15 +154,12 @@
   </si>
   <si>
     <t>2021 4th  Quarter Accomplishment Reports</t>
-  </si>
-  <si>
-    <t>x</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0%"/>
   </numFmts>
@@ -472,12 +483,12 @@
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="72">
+  <cellXfs count="71">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="3" fontId="3" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="4" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="3" fontId="3" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="4" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
@@ -485,36 +496,36 @@
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="15" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="15" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -530,26 +541,23 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="4" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="3" fontId="4" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="2" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="3" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="3" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="3" fontId="4" fillId="3" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -584,11 +592,11 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="3" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="3" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
@@ -599,11 +607,11 @@
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="3" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="3" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
@@ -618,6 +626,21 @@
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -625,6 +648,36 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -640,60 +693,15 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Good" xfId="4" builtinId="26"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="2"/>
-    <cellStyle name="Normal 3" xfId="1"/>
-    <cellStyle name="Percent 2" xfId="3"/>
+    <cellStyle name="Normal 2" xfId="2" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
+    <cellStyle name="Normal 3" xfId="1" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
+    <cellStyle name="Percent 2" xfId="3" xr:uid="{00000000-0005-0000-0000-000004000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -709,9 +717,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -749,9 +757,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -786,7 +794,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -821,7 +829,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -994,11 +1002,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A4:AD14"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A4:AD15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1024,106 +1032,106 @@
   </cols>
   <sheetData>
     <row r="4" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="59" t="s">
-        <v>0</v>
-      </c>
-      <c r="B4" s="59"/>
-      <c r="C4" s="59"/>
-      <c r="D4" s="59"/>
-      <c r="E4" s="59"/>
-      <c r="F4" s="59"/>
-      <c r="G4" s="59"/>
-      <c r="H4" s="59"/>
-      <c r="I4" s="59"/>
-      <c r="J4" s="59"/>
-      <c r="K4" s="59"/>
-      <c r="L4" s="59"/>
-      <c r="M4" s="59"/>
-      <c r="N4" s="59"/>
-      <c r="O4" s="59"/>
-      <c r="P4" s="59"/>
-      <c r="Q4" s="59"/>
-      <c r="R4" s="59"/>
-      <c r="S4" s="59"/>
-      <c r="T4" s="59"/>
-      <c r="U4" s="59"/>
-      <c r="V4" s="59"/>
-      <c r="W4" s="59"/>
-      <c r="X4" s="59"/>
-      <c r="Y4" s="59"/>
-      <c r="Z4" s="59"/>
-      <c r="AA4" s="59"/>
-      <c r="AB4" s="59"/>
-      <c r="AC4" s="59"/>
-      <c r="AD4" s="59"/>
+      <c r="A4" s="48" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" s="48"/>
+      <c r="C4" s="48"/>
+      <c r="D4" s="48"/>
+      <c r="E4" s="48"/>
+      <c r="F4" s="48"/>
+      <c r="G4" s="48"/>
+      <c r="H4" s="48"/>
+      <c r="I4" s="48"/>
+      <c r="J4" s="48"/>
+      <c r="K4" s="48"/>
+      <c r="L4" s="48"/>
+      <c r="M4" s="48"/>
+      <c r="N4" s="48"/>
+      <c r="O4" s="48"/>
+      <c r="P4" s="48"/>
+      <c r="Q4" s="48"/>
+      <c r="R4" s="48"/>
+      <c r="S4" s="48"/>
+      <c r="T4" s="48"/>
+      <c r="U4" s="48"/>
+      <c r="V4" s="48"/>
+      <c r="W4" s="48"/>
+      <c r="X4" s="48"/>
+      <c r="Y4" s="48"/>
+      <c r="Z4" s="48"/>
+      <c r="AA4" s="48"/>
+      <c r="AB4" s="48"/>
+      <c r="AC4" s="48"/>
+      <c r="AD4" s="48"/>
     </row>
     <row r="5" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A5" s="59" t="s">
+      <c r="A5" s="48" t="s">
         <v>38</v>
       </c>
-      <c r="B5" s="59"/>
-      <c r="C5" s="59"/>
-      <c r="D5" s="59"/>
-      <c r="E5" s="59"/>
-      <c r="F5" s="59"/>
-      <c r="G5" s="59"/>
-      <c r="H5" s="59"/>
-      <c r="I5" s="59"/>
-      <c r="J5" s="59"/>
-      <c r="K5" s="59"/>
-      <c r="L5" s="59"/>
-      <c r="M5" s="59"/>
-      <c r="N5" s="59"/>
-      <c r="O5" s="59"/>
-      <c r="P5" s="59"/>
-      <c r="Q5" s="59"/>
-      <c r="R5" s="59"/>
-      <c r="S5" s="59"/>
-      <c r="T5" s="59"/>
-      <c r="U5" s="59"/>
-      <c r="V5" s="59"/>
-      <c r="W5" s="59"/>
-      <c r="X5" s="59"/>
-      <c r="Y5" s="59"/>
-      <c r="Z5" s="59"/>
-      <c r="AA5" s="59"/>
-      <c r="AB5" s="59"/>
-      <c r="AC5" s="59"/>
-      <c r="AD5" s="59"/>
+      <c r="B5" s="48"/>
+      <c r="C5" s="48"/>
+      <c r="D5" s="48"/>
+      <c r="E5" s="48"/>
+      <c r="F5" s="48"/>
+      <c r="G5" s="48"/>
+      <c r="H5" s="48"/>
+      <c r="I5" s="48"/>
+      <c r="J5" s="48"/>
+      <c r="K5" s="48"/>
+      <c r="L5" s="48"/>
+      <c r="M5" s="48"/>
+      <c r="N5" s="48"/>
+      <c r="O5" s="48"/>
+      <c r="P5" s="48"/>
+      <c r="Q5" s="48"/>
+      <c r="R5" s="48"/>
+      <c r="S5" s="48"/>
+      <c r="T5" s="48"/>
+      <c r="U5" s="48"/>
+      <c r="V5" s="48"/>
+      <c r="W5" s="48"/>
+      <c r="X5" s="48"/>
+      <c r="Y5" s="48"/>
+      <c r="Z5" s="48"/>
+      <c r="AA5" s="48"/>
+      <c r="AB5" s="48"/>
+      <c r="AC5" s="48"/>
+      <c r="AD5" s="48"/>
     </row>
     <row r="6" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A6" s="59" t="s">
+      <c r="A6" s="48" t="s">
         <v>39</v>
       </c>
-      <c r="B6" s="59"/>
-      <c r="C6" s="59"/>
-      <c r="D6" s="59"/>
-      <c r="E6" s="59"/>
-      <c r="F6" s="59"/>
-      <c r="G6" s="59"/>
-      <c r="H6" s="59"/>
-      <c r="I6" s="59"/>
-      <c r="J6" s="59"/>
-      <c r="K6" s="59"/>
-      <c r="L6" s="59"/>
-      <c r="M6" s="59"/>
-      <c r="N6" s="59"/>
-      <c r="O6" s="59"/>
-      <c r="P6" s="59"/>
-      <c r="Q6" s="59"/>
-      <c r="R6" s="59"/>
-      <c r="S6" s="59"/>
-      <c r="T6" s="59"/>
-      <c r="U6" s="59"/>
-      <c r="V6" s="59"/>
-      <c r="W6" s="59"/>
-      <c r="X6" s="59"/>
-      <c r="Y6" s="59"/>
-      <c r="Z6" s="59"/>
-      <c r="AA6" s="59"/>
-      <c r="AB6" s="59"/>
-      <c r="AC6" s="59"/>
-      <c r="AD6" s="59"/>
+      <c r="B6" s="48"/>
+      <c r="C6" s="48"/>
+      <c r="D6" s="48"/>
+      <c r="E6" s="48"/>
+      <c r="F6" s="48"/>
+      <c r="G6" s="48"/>
+      <c r="H6" s="48"/>
+      <c r="I6" s="48"/>
+      <c r="J6" s="48"/>
+      <c r="K6" s="48"/>
+      <c r="L6" s="48"/>
+      <c r="M6" s="48"/>
+      <c r="N6" s="48"/>
+      <c r="O6" s="48"/>
+      <c r="P6" s="48"/>
+      <c r="Q6" s="48"/>
+      <c r="R6" s="48"/>
+      <c r="S6" s="48"/>
+      <c r="T6" s="48"/>
+      <c r="U6" s="48"/>
+      <c r="V6" s="48"/>
+      <c r="W6" s="48"/>
+      <c r="X6" s="48"/>
+      <c r="Y6" s="48"/>
+      <c r="Z6" s="48"/>
+      <c r="AA6" s="48"/>
+      <c r="AB6" s="48"/>
+      <c r="AC6" s="48"/>
+      <c r="AD6" s="48"/>
     </row>
     <row r="7" spans="1:30" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="4"/>
@@ -1157,39 +1165,39 @@
       <c r="AD7" s="9"/>
     </row>
     <row r="8" spans="1:30" ht="21" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="60" t="s">
+      <c r="A8" s="49" t="s">
         <v>1</v>
       </c>
-      <c r="B8" s="62" t="s">
+      <c r="B8" s="51" t="s">
         <v>2</v>
       </c>
-      <c r="C8" s="49"/>
-      <c r="D8" s="50"/>
-      <c r="E8" s="50"/>
-      <c r="F8" s="50"/>
-      <c r="G8" s="50"/>
-      <c r="H8" s="50"/>
-      <c r="I8" s="50"/>
-      <c r="J8" s="50"/>
-      <c r="K8" s="50"/>
-      <c r="L8" s="50"/>
-      <c r="M8" s="50"/>
-      <c r="N8" s="50"/>
-      <c r="O8" s="50"/>
-      <c r="P8" s="50"/>
-      <c r="Q8" s="50"/>
-      <c r="R8" s="50"/>
-      <c r="S8" s="50"/>
-      <c r="T8" s="50"/>
-      <c r="U8" s="51"/>
-      <c r="V8" s="64" t="s">
+      <c r="C8" s="53"/>
+      <c r="D8" s="54"/>
+      <c r="E8" s="54"/>
+      <c r="F8" s="54"/>
+      <c r="G8" s="54"/>
+      <c r="H8" s="54"/>
+      <c r="I8" s="54"/>
+      <c r="J8" s="54"/>
+      <c r="K8" s="54"/>
+      <c r="L8" s="54"/>
+      <c r="M8" s="54"/>
+      <c r="N8" s="54"/>
+      <c r="O8" s="54"/>
+      <c r="P8" s="54"/>
+      <c r="Q8" s="54"/>
+      <c r="R8" s="54"/>
+      <c r="S8" s="54"/>
+      <c r="T8" s="54"/>
+      <c r="U8" s="55"/>
+      <c r="V8" s="56" t="s">
         <v>3</v>
       </c>
-      <c r="W8" s="65"/>
-      <c r="X8" s="65"/>
-      <c r="Y8" s="66"/>
+      <c r="W8" s="57"/>
+      <c r="X8" s="57"/>
+      <c r="Y8" s="58"/>
       <c r="Z8" s="19"/>
-      <c r="AA8" s="67" t="s">
+      <c r="AA8" s="59" t="s">
         <v>4</v>
       </c>
       <c r="AB8" s="10"/>
@@ -1197,155 +1205,155 @@
       <c r="AD8" s="21"/>
     </row>
     <row r="9" spans="1:30" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="61"/>
-      <c r="B9" s="63"/>
-      <c r="C9" s="69" t="s">
+      <c r="A9" s="50"/>
+      <c r="B9" s="52"/>
+      <c r="C9" s="61" t="s">
         <v>5</v>
       </c>
-      <c r="D9" s="70"/>
-      <c r="E9" s="71"/>
-      <c r="F9" s="69" t="s">
+      <c r="D9" s="62"/>
+      <c r="E9" s="63"/>
+      <c r="F9" s="61" t="s">
         <v>6</v>
       </c>
-      <c r="G9" s="70"/>
-      <c r="H9" s="71"/>
-      <c r="I9" s="69" t="s">
+      <c r="G9" s="62"/>
+      <c r="H9" s="63"/>
+      <c r="I9" s="61" t="s">
         <v>7</v>
       </c>
-      <c r="J9" s="70"/>
-      <c r="K9" s="70"/>
-      <c r="L9" s="70"/>
-      <c r="M9" s="70"/>
-      <c r="N9" s="71"/>
+      <c r="J9" s="62"/>
+      <c r="K9" s="62"/>
+      <c r="L9" s="62"/>
+      <c r="M9" s="62"/>
+      <c r="N9" s="63"/>
       <c r="O9" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="P9" s="49" t="s">
+      <c r="P9" s="53" t="s">
         <v>9</v>
       </c>
-      <c r="Q9" s="50"/>
-      <c r="R9" s="51"/>
-      <c r="S9" s="52" t="s">
+      <c r="Q9" s="54"/>
+      <c r="R9" s="55"/>
+      <c r="S9" s="66" t="s">
         <v>10</v>
       </c>
-      <c r="T9" s="53"/>
-      <c r="U9" s="54"/>
-      <c r="V9" s="55" t="s">
+      <c r="T9" s="67"/>
+      <c r="U9" s="68"/>
+      <c r="V9" s="69" t="s">
         <v>11</v>
       </c>
-      <c r="W9" s="57" t="s">
+      <c r="W9" s="64" t="s">
         <v>12</v>
       </c>
-      <c r="X9" s="57" t="s">
+      <c r="X9" s="64" t="s">
         <v>13</v>
       </c>
-      <c r="Y9" s="57" t="s">
+      <c r="Y9" s="64" t="s">
         <v>14</v>
       </c>
       <c r="Z9" s="20" t="s">
         <v>37</v>
       </c>
-      <c r="AA9" s="68"/>
+      <c r="AA9" s="60"/>
       <c r="AB9" s="21" t="s">
         <v>15</v>
       </c>
-      <c r="AC9" s="69" t="s">
+      <c r="AC9" s="61" t="s">
         <v>16</v>
       </c>
-      <c r="AD9" s="71"/>
+      <c r="AD9" s="63"/>
     </row>
     <row r="10" spans="1:30" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="61"/>
-      <c r="B10" s="63"/>
-      <c r="C10" s="38" t="s">
+      <c r="A10" s="50"/>
+      <c r="B10" s="52"/>
+      <c r="C10" s="37" t="s">
         <v>17</v>
       </c>
-      <c r="D10" s="23" t="s">
+      <c r="D10" s="22" t="s">
         <v>18</v>
       </c>
-      <c r="E10" s="23" t="s">
+      <c r="E10" s="22" t="s">
         <v>14</v>
       </c>
-      <c r="F10" s="23" t="s">
+      <c r="F10" s="22" t="s">
         <v>19</v>
       </c>
-      <c r="G10" s="23" t="s">
+      <c r="G10" s="22" t="s">
         <v>20</v>
       </c>
-      <c r="H10" s="23" t="s">
+      <c r="H10" s="22" t="s">
         <v>14</v>
       </c>
-      <c r="I10" s="23" t="s">
+      <c r="I10" s="22" t="s">
         <v>21</v>
       </c>
-      <c r="J10" s="23" t="s">
+      <c r="J10" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="K10" s="23" t="s">
+      <c r="K10" s="22" t="s">
         <v>23</v>
       </c>
       <c r="L10" s="22" t="s">
         <v>24</v>
       </c>
-      <c r="M10" s="23" t="s">
+      <c r="M10" s="22" t="s">
         <v>14</v>
       </c>
-      <c r="N10" s="23" t="s">
+      <c r="N10" s="22" t="s">
         <v>25</v>
       </c>
-      <c r="O10" s="39" t="s">
+      <c r="O10" s="38" t="s">
         <v>26</v>
       </c>
-      <c r="P10" s="39" t="s">
+      <c r="P10" s="38" t="s">
         <v>26</v>
       </c>
-      <c r="Q10" s="23" t="s">
+      <c r="Q10" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="R10" s="39" t="s">
+      <c r="R10" s="38" t="s">
         <v>27</v>
       </c>
-      <c r="S10" s="23" t="s">
+      <c r="S10" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="T10" s="23" t="s">
+      <c r="T10" s="22" t="s">
         <v>29</v>
       </c>
-      <c r="U10" s="23" t="s">
+      <c r="U10" s="22" t="s">
         <v>30</v>
       </c>
-      <c r="V10" s="56"/>
-      <c r="W10" s="58"/>
-      <c r="X10" s="58"/>
-      <c r="Y10" s="58"/>
+      <c r="V10" s="70"/>
+      <c r="W10" s="65"/>
+      <c r="X10" s="65"/>
+      <c r="Y10" s="65"/>
       <c r="Z10" s="20"/>
-      <c r="AA10" s="68"/>
-      <c r="AB10" s="23" t="s">
+      <c r="AA10" s="60"/>
+      <c r="AB10" s="22" t="s">
         <v>31</v>
       </c>
-      <c r="AC10" s="23" t="s">
+      <c r="AC10" s="22" t="s">
         <v>32</v>
       </c>
-      <c r="AD10" s="23" t="s">
+      <c r="AD10" s="22" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="11" spans="1:30" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="40" t="s">
+      <c r="A11" s="39" t="s">
         <v>35</v>
       </c>
-      <c r="B11" s="41">
+      <c r="B11" s="40">
         <v>351471</v>
       </c>
       <c r="C11" s="2"/>
       <c r="D11" s="2"/>
-      <c r="E11" s="42">
-        <f t="shared" ref="E11:E13" si="0">C11+D11</f>
+      <c r="E11" s="41">
+        <f t="shared" ref="E11:E14" si="0">C11+D11</f>
         <v>0</v>
       </c>
       <c r="F11" s="2"/>
       <c r="G11" s="2"/>
-      <c r="H11" s="42">
+      <c r="H11" s="41">
         <f t="shared" ref="H11" si="1">F11+G11</f>
         <v>0</v>
       </c>
@@ -1356,8 +1364,8 @@
         <f t="shared" ref="L11:L12" si="2">J11+K11</f>
         <v>0</v>
       </c>
-      <c r="M11" s="42">
-        <f t="shared" ref="M11:M12" si="3">I11+J11+K11</f>
+      <c r="M11" s="41">
+        <f t="shared" ref="M11:M13" si="3">I11+J11+K11</f>
         <v>0</v>
       </c>
       <c r="N11" s="13"/>
@@ -1371,206 +1379,258 @@
       <c r="V11" s="2"/>
       <c r="W11" s="2"/>
       <c r="X11" s="2"/>
-      <c r="Y11" s="43">
+      <c r="Y11" s="42">
         <f>V11+W11+X11</f>
         <v>0</v>
       </c>
-      <c r="Z11" s="43"/>
+      <c r="Z11" s="42"/>
       <c r="AA11" s="2"/>
       <c r="AB11" s="16"/>
       <c r="AC11" s="12" t="e">
-        <f t="shared" ref="AC11:AC12" si="4">S11/L11</f>
+        <f t="shared" ref="AC11:AC13" si="4">S11/L11</f>
         <v>#DIV/0!</v>
       </c>
       <c r="AD11" s="12" t="e">
-        <f t="shared" ref="AD11:AD12" si="5">(T11+U11)/K11</f>
+        <f t="shared" ref="AD11:AD13" si="5">(T11+U11)/K11</f>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="12" spans="1:30" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="44" t="s">
+    <row r="12" spans="1:30" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="43" t="s">
         <v>36</v>
       </c>
-      <c r="B12" s="45">
+      <c r="B12" s="44">
         <v>18401</v>
       </c>
-      <c r="C12" s="24"/>
-      <c r="D12" s="24"/>
-      <c r="E12" s="46">
+      <c r="C12" s="23"/>
+      <c r="D12" s="23"/>
+      <c r="E12" s="45">
         <f>C12+D12</f>
         <v>0</v>
       </c>
-      <c r="F12" s="24"/>
-      <c r="G12" s="24"/>
-      <c r="H12" s="46">
+      <c r="F12" s="23"/>
+      <c r="G12" s="23"/>
+      <c r="H12" s="45">
         <f>F12+G12</f>
         <v>0</v>
       </c>
-      <c r="I12" s="24"/>
-      <c r="J12" s="24"/>
-      <c r="K12" s="24"/>
+      <c r="I12" s="23"/>
+      <c r="J12" s="23"/>
+      <c r="K12" s="23"/>
       <c r="L12" s="17">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="M12" s="46">
+      <c r="M12" s="45">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="N12" s="27"/>
-      <c r="O12" s="28"/>
-      <c r="P12" s="29"/>
+      <c r="N12" s="26"/>
+      <c r="O12" s="27"/>
+      <c r="P12" s="28"/>
       <c r="Q12" s="17"/>
       <c r="R12" s="17"/>
-      <c r="S12" s="30"/>
-      <c r="T12" s="47"/>
-      <c r="U12" s="47"/>
-      <c r="V12" s="47"/>
-      <c r="W12" s="47"/>
-      <c r="X12" s="47"/>
-      <c r="Y12" s="48">
+      <c r="S12" s="29"/>
+      <c r="T12" s="46"/>
+      <c r="U12" s="46"/>
+      <c r="V12" s="46"/>
+      <c r="W12" s="46"/>
+      <c r="X12" s="46"/>
+      <c r="Y12" s="47">
         <f>V12+W12+X12</f>
         <v>0</v>
       </c>
-      <c r="Z12" s="48"/>
-      <c r="AA12" s="24"/>
-      <c r="AB12" s="25"/>
-      <c r="AC12" s="26" t="e">
+      <c r="Z12" s="47"/>
+      <c r="AA12" s="23"/>
+      <c r="AB12" s="24"/>
+      <c r="AC12" s="25" t="e">
         <f t="shared" si="4"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="AD12" s="26" t="e">
+      <c r="AD12" s="25" t="e">
         <f t="shared" si="5"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="13" spans="1:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="31" t="s">
+    <row r="13" spans="1:30" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="43"/>
+      <c r="B13" s="44"/>
+      <c r="C13" s="23"/>
+      <c r="D13" s="23"/>
+      <c r="E13" s="45">
+        <f>C13+D13</f>
+        <v>0</v>
+      </c>
+      <c r="F13" s="23"/>
+      <c r="G13" s="23"/>
+      <c r="H13" s="45">
+        <f>F13+G13</f>
+        <v>0</v>
+      </c>
+      <c r="I13" s="23"/>
+      <c r="J13" s="23"/>
+      <c r="K13" s="23"/>
+      <c r="L13" s="45">
+        <f>J13+K13</f>
+        <v>0</v>
+      </c>
+      <c r="M13" s="45">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="N13" s="26"/>
+      <c r="O13" s="27"/>
+      <c r="P13" s="28"/>
+      <c r="Q13" s="17"/>
+      <c r="R13" s="17"/>
+      <c r="S13" s="29"/>
+      <c r="T13" s="46"/>
+      <c r="U13" s="46"/>
+      <c r="V13" s="46"/>
+      <c r="W13" s="46"/>
+      <c r="X13" s="46"/>
+      <c r="Y13" s="47">
+        <f>V13+W13+X13</f>
+        <v>0</v>
+      </c>
+      <c r="Z13" s="47"/>
+      <c r="AA13" s="23"/>
+      <c r="AB13" s="24"/>
+      <c r="AC13" s="25" t="e">
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AD13" s="25" t="e">
+        <f t="shared" si="5"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="14" spans="1:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="30" t="s">
         <v>34</v>
       </c>
-      <c r="B13" s="32">
+      <c r="B14" s="31">
         <f>SUM(B11:B12)</f>
         <v>369872</v>
       </c>
-      <c r="C13" s="32">
-        <f>SUM(C11:C12)</f>
-        <v>0</v>
-      </c>
-      <c r="D13" s="32">
-        <f>SUM(D11:D12)</f>
-        <v>0</v>
-      </c>
-      <c r="E13" s="32">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F13" s="32">
-        <f t="shared" ref="F13:M13" si="6">SUM(F11:F12)</f>
-        <v>0</v>
-      </c>
-      <c r="G13" s="32">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="H13" s="32">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="I13" s="32">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="J13" s="32">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="K13" s="32">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="L13" s="32">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="M13" s="32">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="N13" s="33"/>
-      <c r="O13" s="34"/>
-      <c r="P13" s="32">
-        <f>SUM(P11:P12)</f>
-        <v>0</v>
-      </c>
-      <c r="Q13" s="32">
-        <f>SUM(Q11:Q12)</f>
-        <v>0</v>
-      </c>
-      <c r="R13" s="32"/>
-      <c r="S13" s="32">
-        <f t="shared" ref="S13:X13" si="7">SUM(S11:S12)</f>
-        <v>0</v>
-      </c>
-      <c r="T13" s="32">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="U13" s="32">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="V13" s="32">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="W13" s="32">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="X13" s="32">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="Y13" s="35">
-        <f>V13+W13+X13</f>
-        <v>0</v>
-      </c>
-      <c r="Z13" s="35">
-        <f>SUM(Z11:Z12)</f>
-        <v>0</v>
-      </c>
-      <c r="AA13" s="35">
-        <f>SUM(AA11:AA12)</f>
-        <v>0</v>
-      </c>
-      <c r="AB13" s="36"/>
-      <c r="AC13" s="37" t="e">
-        <f>S13/(J13+K13)</f>
+      <c r="C14" s="31">
+        <f>SUM(C11:C13)</f>
+        <v>0</v>
+      </c>
+      <c r="D14" s="31">
+        <f>SUM(D11:D13)</f>
+        <v>0</v>
+      </c>
+      <c r="E14" s="31">
+        <f>C14+D14</f>
+        <v>0</v>
+      </c>
+      <c r="F14" s="31">
+        <f>SUM(F11:F13)</f>
+        <v>0</v>
+      </c>
+      <c r="G14" s="31">
+        <f>SUM(G11:G13)</f>
+        <v>0</v>
+      </c>
+      <c r="H14" s="31">
+        <f>SUM(H11:H13)</f>
+        <v>0</v>
+      </c>
+      <c r="I14" s="31">
+        <f>SUM(I11:I13)</f>
+        <v>0</v>
+      </c>
+      <c r="J14" s="31">
+        <f>SUM(J11:J13)</f>
+        <v>0</v>
+      </c>
+      <c r="K14" s="31">
+        <f>SUM(K11:K13)</f>
+        <v>0</v>
+      </c>
+      <c r="L14" s="31">
+        <f>SUM(L11:L13)</f>
+        <v>0</v>
+      </c>
+      <c r="M14" s="31">
+        <f>SUM(M11:O13)</f>
+        <v>0</v>
+      </c>
+      <c r="N14" s="32"/>
+      <c r="O14" s="33"/>
+      <c r="P14" s="31">
+        <f>SUM(P11:P13)</f>
+        <v>0</v>
+      </c>
+      <c r="Q14" s="31">
+        <f>SUM(Q11:Q13)</f>
+        <v>0</v>
+      </c>
+      <c r="R14" s="31"/>
+      <c r="S14" s="31">
+        <f>SUM(S11:S13)</f>
+        <v>0</v>
+      </c>
+      <c r="T14" s="31">
+        <f>SUM(T11:T13)</f>
+        <v>0</v>
+      </c>
+      <c r="U14" s="31">
+        <f>SUM(U11:U13)</f>
+        <v>0</v>
+      </c>
+      <c r="V14" s="31">
+        <f>SUM(V11:V13)</f>
+        <v>0</v>
+      </c>
+      <c r="W14" s="31">
+        <f>SUM(W11:W13)</f>
+        <v>0</v>
+      </c>
+      <c r="X14" s="31">
+        <f>SUM(X11:X13)</f>
+        <v>0</v>
+      </c>
+      <c r="Y14" s="34">
+        <f>V14+W14+X14</f>
+        <v>0</v>
+      </c>
+      <c r="Z14" s="34">
+        <f>SUM(Z11:Z13)</f>
+        <v>0</v>
+      </c>
+      <c r="AA14" s="34">
+        <f>SUM(AA11:AA13)</f>
+        <v>0</v>
+      </c>
+      <c r="AB14" s="35"/>
+      <c r="AC14" s="36" t="e">
+        <f>S14/(J14+K14)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="AD13" s="37" t="e">
-        <f>(T13+U13)/K13</f>
+      <c r="AD14" s="36" t="e">
+        <f>(T14+U14)/K14</f>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="14" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="H14" t="s">
-        <v>40</v>
-      </c>
-      <c r="J14" s="18"/>
-      <c r="K14" s="18"/>
-      <c r="L14" s="18"/>
-      <c r="M14" s="18"/>
-      <c r="T14" s="18"/>
-      <c r="U14" s="18"/>
-      <c r="V14" s="18"/>
-      <c r="W14" s="18"/>
-      <c r="X14" s="18"/>
-      <c r="Y14" s="18"/>
-      <c r="Z14" s="18"/>
+    <row r="15" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="J15" s="18"/>
+      <c r="K15" s="18"/>
+      <c r="L15" s="18"/>
+      <c r="M15" s="18"/>
+      <c r="T15" s="18"/>
+      <c r="U15" s="18"/>
+      <c r="V15" s="18"/>
+      <c r="W15" s="18"/>
+      <c r="X15" s="18"/>
+      <c r="Y15" s="18"/>
+      <c r="Z15" s="18"/>
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="W9:W10"/>
+    <mergeCell ref="X9:X10"/>
     <mergeCell ref="A4:AD4"/>
     <mergeCell ref="A5:AD5"/>
     <mergeCell ref="A6:AD6"/>
@@ -1587,8 +1647,6 @@
     <mergeCell ref="P9:R9"/>
     <mergeCell ref="S9:U9"/>
     <mergeCell ref="V9:V10"/>
-    <mergeCell ref="W9:W10"/>
-    <mergeCell ref="X9:X10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>